<commit_message>
add lot yield to tooltip
</commit_message>
<xml_diff>
--- a/data/addresses.xlsx
+++ b/data/addresses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbuck/Desktop/NMP/MAP673/BlightedToBountiful/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F018492-8204-E24A-A360-F3F49AF16CAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E603CBF-45E9-164D-A23D-E4B4ECDE75E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{9123AF10-BEF5-F743-AFF6-F8B1E991249B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{9123AF10-BEF5-F743-AFF6-F8B1E991249B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -279,6 +279,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -349,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -373,6 +376,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,7 +694,7 @@
   <dimension ref="A1:Y54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="G2" sqref="G2:G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -797,7 +801,7 @@
       <c r="F2" s="7">
         <v>140000</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="11">
         <v>0.5</v>
       </c>
       <c r="H2" s="9">
@@ -874,7 +878,7 @@
       <c r="F3" s="7">
         <v>14100</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="11">
         <v>0.5</v>
       </c>
       <c r="H3" s="9">
@@ -951,7 +955,7 @@
       <c r="F4" s="7">
         <v>586400</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="11">
         <v>0.5</v>
       </c>
       <c r="H4" s="9">
@@ -1028,7 +1032,7 @@
       <c r="F5" s="7">
         <v>211600</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="11">
         <v>0.5</v>
       </c>
       <c r="H5" s="9">
@@ -1105,7 +1109,7 @@
       <c r="F6" s="7">
         <v>162500</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="11">
         <v>0.5</v>
       </c>
       <c r="H6" s="9">
@@ -1182,7 +1186,7 @@
       <c r="F7" s="7">
         <v>16100</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="11">
         <v>0.5</v>
       </c>
       <c r="H7" s="9">
@@ -1259,7 +1263,7 @@
       <c r="F8" s="7">
         <v>65000</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="11">
         <v>0.5</v>
       </c>
       <c r="H8" s="9">
@@ -1336,7 +1340,7 @@
       <c r="F9" s="7">
         <v>667400</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="11">
         <v>0.5</v>
       </c>
       <c r="H9" s="9">
@@ -1413,7 +1417,7 @@
       <c r="F10" s="7">
         <v>155800</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="11">
         <v>0.5</v>
       </c>
       <c r="H10" s="9">
@@ -1490,7 +1494,7 @@
       <c r="F11" s="7">
         <v>331500</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="11">
         <v>0.5</v>
       </c>
       <c r="H11" s="9">
@@ -1567,7 +1571,7 @@
       <c r="F12" s="7">
         <v>9500</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="11">
         <v>0.5</v>
       </c>
       <c r="H12" s="9">
@@ -1644,7 +1648,7 @@
       <c r="F13" s="7">
         <v>16500</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="11">
         <v>0.5</v>
       </c>
       <c r="H13" s="9">
@@ -1721,7 +1725,7 @@
       <c r="F14" s="7">
         <v>291500</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="11">
         <v>0.5</v>
       </c>
       <c r="H14" s="9">
@@ -1798,7 +1802,7 @@
       <c r="F15" s="7">
         <v>17000</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="11">
         <v>0.5</v>
       </c>
       <c r="H15" s="9">
@@ -1875,7 +1879,7 @@
       <c r="F16" s="7">
         <v>19600</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="11">
         <v>0.5</v>
       </c>
       <c r="H16" s="9">
@@ -1952,7 +1956,7 @@
       <c r="F17" s="7">
         <v>19600</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="11">
         <v>0.5</v>
       </c>
       <c r="H17" s="9">
@@ -2029,7 +2033,7 @@
       <c r="F18" s="7">
         <v>17000</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="11">
         <v>0.5</v>
       </c>
       <c r="H18" s="9">
@@ -2106,7 +2110,7 @@
       <c r="F19" s="7">
         <v>25000</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="11">
         <v>0.5</v>
       </c>
       <c r="H19" s="9">
@@ -2183,7 +2187,7 @@
       <c r="F20" s="7">
         <v>10800</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="11">
         <v>0.5</v>
       </c>
       <c r="H20" s="9">
@@ -2260,7 +2264,7 @@
       <c r="F21" s="7">
         <v>21300</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="11">
         <v>0.5</v>
       </c>
       <c r="H21" s="9">
@@ -2337,7 +2341,7 @@
       <c r="F22" s="7">
         <v>15300</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="11">
         <v>0.5</v>
       </c>
       <c r="H22" s="9">
@@ -2414,7 +2418,7 @@
       <c r="F23" s="7">
         <v>18700</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="11">
         <v>0.5</v>
       </c>
       <c r="H23" s="9">
@@ -2491,7 +2495,7 @@
       <c r="F24" s="7">
         <v>82900</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="11">
         <v>0.5</v>
       </c>
       <c r="H24" s="9">
@@ -2568,7 +2572,7 @@
       <c r="F25" s="7">
         <v>44600</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="11">
         <v>0.5</v>
       </c>
       <c r="H25" s="9">
@@ -2645,7 +2649,7 @@
       <c r="F26" s="7">
         <v>80400</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="11">
         <v>0.5</v>
       </c>
       <c r="H26" s="9">
@@ -2722,7 +2726,7 @@
       <c r="F27" s="7">
         <v>24600</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="11">
         <v>0.5</v>
       </c>
       <c r="H27" s="9">
@@ -2799,7 +2803,7 @@
       <c r="F28" s="7">
         <v>1386900</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="11">
         <v>0.5</v>
       </c>
       <c r="H28" s="9">
@@ -2876,7 +2880,7 @@
       <c r="F29" s="7">
         <v>22000</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="11">
         <v>0.5</v>
       </c>
       <c r="H29" s="9">
@@ -2953,7 +2957,7 @@
       <c r="F30" s="7">
         <v>50000</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="11">
         <v>0.5</v>
       </c>
       <c r="H30" s="9">
@@ -3030,7 +3034,7 @@
       <c r="F31" s="7">
         <v>24000</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="11">
         <v>0.5</v>
       </c>
       <c r="H31" s="9">
@@ -3107,7 +3111,7 @@
       <c r="F32" s="7">
         <v>136500</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="11">
         <v>0.5</v>
       </c>
       <c r="H32" s="9">
@@ -3184,7 +3188,7 @@
       <c r="F33" s="7">
         <v>157900</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="11">
         <v>0.5</v>
       </c>
       <c r="H33" s="9">
@@ -3261,7 +3265,7 @@
       <c r="F34" s="7">
         <v>122600</v>
       </c>
-      <c r="G34" s="9">
+      <c r="G34" s="11">
         <v>0.5</v>
       </c>
       <c r="H34" s="9">
@@ -3338,7 +3342,7 @@
       <c r="F35" s="7">
         <v>132100</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="11">
         <v>0.5</v>
       </c>
       <c r="H35" s="9">
@@ -3415,7 +3419,7 @@
       <c r="F36" s="7">
         <v>51000</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="11">
         <v>0.5</v>
       </c>
       <c r="H36" s="9">
@@ -3492,7 +3496,7 @@
       <c r="F37" s="7">
         <v>51000</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="11">
         <v>0.5</v>
       </c>
       <c r="H37" s="9">
@@ -3569,7 +3573,7 @@
       <c r="F38" s="7">
         <v>170500</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="11">
         <v>0.5</v>
       </c>
       <c r="H38" s="9">
@@ -3646,7 +3650,7 @@
       <c r="F39" s="7">
         <v>134100</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="11">
         <v>0.5</v>
       </c>
       <c r="H39" s="9">
@@ -3723,7 +3727,7 @@
       <c r="F40" s="7">
         <v>137800</v>
       </c>
-      <c r="G40" s="9">
+      <c r="G40" s="11">
         <v>0.5</v>
       </c>
       <c r="H40" s="9">
@@ -3800,7 +3804,7 @@
       <c r="F41" s="7">
         <v>20000</v>
       </c>
-      <c r="G41" s="9">
+      <c r="G41" s="11">
         <v>0.5</v>
       </c>
       <c r="H41" s="9">
@@ -3877,7 +3881,7 @@
       <c r="F42" s="7">
         <v>14500</v>
       </c>
-      <c r="G42" s="9">
+      <c r="G42" s="11">
         <v>0.5</v>
       </c>
       <c r="H42" s="9">
@@ -3954,7 +3958,7 @@
       <c r="F43" s="7">
         <v>1300</v>
       </c>
-      <c r="G43" s="9">
+      <c r="G43" s="11">
         <v>0.5</v>
       </c>
       <c r="H43" s="9">
@@ -4031,7 +4035,7 @@
       <c r="F44" s="7">
         <v>430200</v>
       </c>
-      <c r="G44" s="9">
+      <c r="G44" s="11">
         <v>0.5</v>
       </c>
       <c r="H44" s="9">
@@ -4108,7 +4112,7 @@
       <c r="F45" s="7">
         <v>22000</v>
       </c>
-      <c r="G45" s="9">
+      <c r="G45" s="11">
         <v>0.5</v>
       </c>
       <c r="H45" s="9">
@@ -4185,7 +4189,7 @@
       <c r="F46" s="7">
         <v>6600</v>
       </c>
-      <c r="G46" s="9">
+      <c r="G46" s="11">
         <v>0.5</v>
       </c>
       <c r="H46" s="9">
@@ -4262,7 +4266,7 @@
       <c r="F47" s="7">
         <v>111900</v>
       </c>
-      <c r="G47" s="9">
+      <c r="G47" s="11">
         <v>0.5</v>
       </c>
       <c r="H47" s="9">
@@ -4339,7 +4343,7 @@
       <c r="F48" s="7">
         <v>51000</v>
       </c>
-      <c r="G48" s="9">
+      <c r="G48" s="11">
         <v>0.5</v>
       </c>
       <c r="H48" s="9">
@@ -4416,7 +4420,7 @@
       <c r="F49" s="7">
         <v>32800</v>
       </c>
-      <c r="G49" s="9">
+      <c r="G49" s="11">
         <v>0.5</v>
       </c>
       <c r="H49" s="9">
@@ -4493,7 +4497,7 @@
       <c r="F50" s="7">
         <v>104000</v>
       </c>
-      <c r="G50" s="9">
+      <c r="G50" s="11">
         <v>0.5</v>
       </c>
       <c r="H50" s="9">
@@ -4570,7 +4574,7 @@
       <c r="F51" s="7">
         <v>89800</v>
       </c>
-      <c r="G51" s="9">
+      <c r="G51" s="11">
         <v>0.5</v>
       </c>
       <c r="H51" s="9">
@@ -4647,7 +4651,7 @@
       <c r="F52" s="7">
         <v>149800</v>
       </c>
-      <c r="G52" s="9">
+      <c r="G52" s="11">
         <v>0.5</v>
       </c>
       <c r="H52" s="9">
@@ -4724,7 +4728,7 @@
       <c r="F53" s="7">
         <v>105200</v>
       </c>
-      <c r="G53" s="9">
+      <c r="G53" s="11">
         <v>0.5</v>
       </c>
       <c r="H53" s="9">
@@ -4801,7 +4805,7 @@
       <c r="F54" s="7">
         <v>20000</v>
       </c>
-      <c r="G54" s="9">
+      <c r="G54" s="11">
         <v>0.5</v>
       </c>
       <c r="H54" s="9">

</xml_diff>

<commit_message>
fix map <iframe> in tooltip
</commit_message>
<xml_diff>
--- a/data/addresses.xlsx
+++ b/data/addresses.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbuck/Desktop/NMP/MAP673/BlightedToBountiful/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B74FCAC-DC90-864C-A025-F5AFC8AA13FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B9869C-9ABB-8748-A12B-ED3696298CA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{9123AF10-BEF5-F743-AFF6-F8B1E991249B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{9123AF10-BEF5-F743-AFF6-F8B1E991249B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="128">
   <si>
     <t>address</t>
   </si>
@@ -272,33 +273,9 @@
     <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.308684341667&amp;y=36.8791583084625</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/@36.8764086,-76.3021443,3a,73.7y,206.12h,77.85t/data=!3m6!1e1!3m4!1s8U-ZeWwm6X4Kdo4BNSCpOA!2e0!7i16384!8i8192</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/@36.8770493,-76.3044719,3a,90y,142.83h,76.45t/data=!3m7!1e1!3m5!1sAF1QipPzJOt4XLT8XEQaRG-b_ThxJ3bQ7UDZyhlhzr7m!2e10!3e12!7i5760!8i2880</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/@36.8741587,-76.2914247,3a,73.7y,55.95h,80.41t/data=!3m6!1e1!3m4!1symIK2jpp-xvGR-nO60cKZw!2e0!7i13312!8i6656</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/@36.8753677,-76.2903392,3a,56.4y,213.77h,92.77t/data=!3m6!1e1!3m4!1swcUVQh-wprUtYMecIvLInA!2e0!7i16384!8i8192</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/2612+Monticello+Ave,+Norfolk,+VA+23517/@36.8706106,-76.282217,3a,75y,26.37h,89.1t/data=!3m7!1e1!3m5!1sJm_WmtqCPNdIJ5VpTd1Abw!2e0!6s%2F%2Fgeo2.ggpht.com%2Fcbk%3Fpanoid%3DJm_WmtqCPNdIJ5VpTd1Abw%26output%3Dthumbnail%26cb_client%3Dsearch.gws-prod.gps%26thumb%3D2%26w%3D86%26h%3D86%26yaw%3D357.51123%26pitch%3D0%26thumbfov%3D100!7i13312!8i6656!4m5!3m4!1s0x89ba98254e888bd5:0xd3314741a1a16105!8m2!3d36.8707309!4d-76.282256</t>
-  </si>
-  <si>
     <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2975126025031&amp;y=36.8746790155474</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/place/2000+Church+St,+Norfolk,+VA+23504/@36.866342,-76.2788727,3a,38.2y,102.92h,87.97t/data=!3m6!1e1!3m4!1sh7_Udt5sNqGgjBlP79uepw!2e0!7i16384!8i8192!4m5!3m4!1s0x89ba982412940d9f:0xfc7b0d76d737b97c!8m2!3d36.86654!4d-76.2782129</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/2433+Hale+St,+Norfolk,+VA+23504/@36.8693219,-76.2753233,3a,75y,253.21h,91.54t/data=!3m6!1e1!3m4!1sYCfmlHrVa8XlFUiJ5qmSVg!2e0!7i16384!8i8192!4m5!3m4!1s0x89ba98266614a029:0xfb52772367006d3!8m2!3d36.8687438!4d-76.2757211</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/@36.8640759,-76.2663241,3a,90y,209.64h,74.9t/data=!3m6!1e1!3m4!1sPH5yNpIXm7SFjUH8ImahpA!2e0!7i13312!8i6656</t>
-  </si>
-  <si>
     <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2723602254643&amp;y=36.8579139694955</t>
   </si>
   <si>
@@ -335,12 +312,6 @@
     <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2525436931686&amp;y=36.8521261987788</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/@36.85485,-76.2674651,3a,73.7y,86.52h,75.63t/data=!3m6!1e1!3m4!1snil0JjNqx458FLnteaCptA!2e0!7i16384!8i8192</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/930+E+Virginia+Beach+Blvd,+Norfolk,+VA+23504/@36.8546596,-76.2749356,3a,90y,358.8h,87.93t/data=!3m6!1e1!3m4!1so68-ruh7cZGBxnC2c5gdDw!2e0!7i16384!8i8192!4m5!3m4!1s0x89ba981e9a18a563:0xfed0c4efcdd81481!8m2!3d36.855462!4d-76.27504</t>
-  </si>
-  <si>
     <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2501842085679&amp;y=36.8632022029132</t>
   </si>
   <si>
@@ -368,42 +339,18 @@
     <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.262616655931&amp;y=36.9168803738438</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/@36.9158979,-76.2631474,3a,75y,359h,86.4t/data=!3m7!1e1!3m5!1sQlaeuGuu5OwZHIxyA_TW7g!2e0!6s%2F%2Fgeo3.ggpht.com%2Fcbk%3Fpanoid%3DQlaeuGuu5OwZHIxyA_TW7g%26output%3Dthumbnail%26cb_client%3Dmaps_sv.tactile.gps%26thumb%3D2%26w%3D203%26h%3D100%26yaw%3D292.73462%26pitch%3D0%26thumbfov%3D100!7i16384!8i8192</t>
-  </si>
-  <si>
     <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2950852234906&amp;y=36.9164763650166</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/@36.8783273,-76.299252,3a,50.6y,180.9h,90.17t/data=!3m6!1e1!3m4!1sNT6JL8kwzmwiW6tEcboPMw!2e0!7i16384!8i8192</t>
-  </si>
-  <si>
     <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2912710468707&amp;y=36.8742703307802</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/place/1310+Olinger+St,+Norfolk,+VA+23523/@36.8336179,-76.2637123,3a,75y,320.45h,84.71t/data=!3m6!1e1!3m4!1skUrI4l82XW1y9YTSS6wRJQ!2e0!7i3328!8i1664!4m5!3m4!1s0x89babd56953eb255:0xd3aa7daaa82e2661!8m2!3d36.8338745!4d-76.2639113</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/place/1418+Ballentine+Blvd,+Norfolk,+VA+23504/@36.8593939,-76.2496023,3a,74.9y,75.18h,99.64t/data=!3m7!1e1!3m5!1sfWED1BsjWb_y3zyUmXEbUg!2e0!6s%2F%2Fgeo3.ggpht.com%2Fcbk%3Fpanoid%3DfWED1BsjWb_y3zyUmXEbUg%26output%3Dthumbnail%26cb_client%3Dsearch.gws-prod.gps%26thumb%3D2%26w%3D86%26h%3D86%26yaw%3D74.78842%26pitch%3D0%26thumbfov%3D100!7i16384!8i8192!4m5!3m4!1s0x89ba97959d6de8f5:0x2b0cbdf6cc0bf3fa!8m2!3d36.85963!4d-76.249023</t>
-  </si>
-  <si>
     <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2480788400734&amp;y=36.878018532031</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/@36.8876382,-76.2156766,3a,90y,225.71h,71.42t/data=!3m6!1e1!3m4!1sSAowHANp1loT7OdLHiMHKQ!2e0!7i13312!8i6656</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/@36.9180283,-76.2639314,3a,90y,145.48h,93.81t/data=!3m6!1e1!3m4!1sXqFjvXGVn4nw-yXEuUESGw!2e0!7i16384!8i8192</t>
-  </si>
-  <si>
     <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.263639502536&amp;y=36.9174739008572</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/@36.9162938,-76.2652523,3a,73.7y,5.48h,90.85t/data=!3m6!1e1!3m4!1sQ61TNKdBRCldH42QpXRaeQ!2e0!7i16384!8i8192</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps/@36.916057,-76.2647943,3a,75y,20.16h,95.19t/data=!3m6!1e1!3m4!1sn02BncmaPSzSnv5Bc6oXRg!2e0!7i16384!8i8192</t>
-  </si>
-  <si>
     <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2648470984892&amp;y=36.916414116563</t>
   </si>
   <si>
@@ -416,7 +363,61 @@
     <t>streetView</t>
   </si>
   <si>
-    <t>https://goo.gl/maps/FrZo4oawDTkEjZLs8</t>
+    <t>https://www.google.com/maps/embed?pb=!4v1591898714655!6m8!1m7!1s8U-ZeWwm6X4Kdo4BNSCpOA!2m2!1d36.87640858420767!2d-76.30214434531852!3f206.12!4f-12.150000000000006!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591898832477!6m8!1m7!1sL54lMXjuywAuomeLIi35KQ!2m2!1d36.87727018639783!2d-76.30231861662762!3f193.08!4f-9.239999999999995!5f0.7820865974627469</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591899281313!6m8!1m7!1sCAoSLEFGMVFpcFB6Sk90NFhMVDhYRVFhUkctYl9UaHhKM2JRN1VEWnlobGh6cjdt!2m2!1d36.87704929135312!2d-76.30447188644887!3f142.83!4f-13.549999999999997!5f0.4000000000000002</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591899553932!6m8!1m7!1symIK2jpp-xvGR-nO60cKZw!2m2!1d36.87415872183867!2d-76.2914247034883!3f55.95!4f-9.590000000000003!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591899636665!6m8!1m7!1swcUVQh-wprUtYMecIvLInA!2m2!1d36.87536774264987!2d-76.2903391663852!3f213.77!4f2.769999999999996!5f1.299169533619291</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591899687956!6m8!1m7!1sJm_WmtqCPNdIJ5VpTd1Abw!2m2!1d36.87061059820953!2d-76.28221700521999!3f26.37!4f-0.9000000000000057!5f0.7820865974627469</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591899743574!6m8!1m7!1sh7_Udt5sNqGgjBlP79uepw!2m2!1d36.86634202358129!2d-76.27887267230223!3f102.92!4f-2.030000000000001!5f1.9299846668249203</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591899806954!6m8!1m7!1sYCfmlHrVa8XlFUiJ5qmSVg!2m2!1d36.86932186268548!2d-76.27532325866841!3f253.21!4f1.5400000000000063!5f0.7820865974627469</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591899881481!6m8!1m7!1sPH5yNpIXm7SFjUH8ImahpA!2m2!1d36.86407592000155!2d-76.26632411329217!3f209.64!4f-15.099999999999994!5f0.4000000000000002</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591899946149!6m8!1m7!1snil0JjNqx458FLnteaCptA!2m2!1d36.85485000394906!2d-76.26746511883589!3f86.52!4f-14.370000000000005!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591900119798!6m8!1m7!1so68-ruh7cZGBxnC2c5gdDw!2m2!1d36.85465958010599!2d-76.27493555751877!3f358.8!4f-2.069999999999993!5f0.4000000000000002</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591900202232!6m8!1m7!1sQlaeuGuu5OwZHIxyA_TW7g!2m2!1d36.91589788837648!2d-76.2631473532459!3f359!4f-3.5999999999999943!5f0.7820865974627469</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591900247479!6m8!1m7!1sNT6JL8kwzmwiW6tEcboPMw!2m2!1d36.87832725295541!2d-76.29925195553068!3f180.9!4f0.1700000000000017!5f1.4810098395366498</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591900298211!6m8!1m7!1skUrI4l82XW1y9YTSS6wRJQ!2m2!1d36.83361787748391!2d-76.2637123397932!3f320.45!4f-5.290000000000006!5f0.7820865974627469</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591900346065!6m8!1m7!1sfWED1BsjWb_y3zyUmXEbUg!2m2!1d36.85939385951343!2d-76.24960226498114!3f75.18!4f9.64!5f0.7846940110228585</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591900395253!6m8!1m7!1sSAowHANp1loT7OdLHiMHKQ!2m2!1d36.8876382449219!2d-76.21567660401722!3f225.71!4f-18.58!5f0.4000000000000002</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591900435973!6m8!1m7!1sXqFjvXGVn4nw-yXEuUESGw!2m2!1d36.91802827499728!2d-76.26393139607409!3f145.48!4f3.8100000000000023!5f0.4000000000000002</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591900485980!6m8!1m7!1sQ61TNKdBRCldH42QpXRaeQ!2m2!1d36.91629375536341!2d-76.26525228074574!3f5.48!4f0.8499999999999943!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1591900531258!6m8!1m7!1sn02BncmaPSzSnv5Bc6oXRg!2m2!1d36.91605702410043!2d-76.26479426860529!3f20.16!4f5.189999999999998!5f0.7820865974627469</t>
   </si>
 </sst>
 </file>
@@ -426,7 +427,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -453,6 +454,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -505,7 +512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -532,6 +539,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -850,7 +858,7 @@
   <dimension ref="A1:Z51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Z4" sqref="Z4"/>
+      <selection activeCell="Y48" sqref="Y48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -942,7 +950,7 @@
         <v>76</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -1020,7 +1028,7 @@
       <c r="X2" s="10">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" s="9">
         <v>6560800</v>
       </c>
       <c r="Z2" s="13" t="s">
@@ -1102,7 +1110,7 @@
       <c r="X3">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y3">
+      <c r="Y3" s="9">
         <v>6560800</v>
       </c>
       <c r="Z3" s="13" t="s">
@@ -1184,11 +1192,11 @@
       <c r="X4">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="9">
         <v>6560800</v>
       </c>
       <c r="Z4" s="13" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
@@ -1266,11 +1274,11 @@
       <c r="X5" s="10">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y5">
+      <c r="Y5" s="9">
         <v>6560800</v>
       </c>
       <c r="Z5" s="13" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
@@ -1348,11 +1356,11 @@
       <c r="X6">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y6">
+      <c r="Y6" s="9">
         <v>6560800</v>
       </c>
       <c r="Z6" s="13" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
@@ -1430,11 +1438,11 @@
       <c r="X7">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y7">
+      <c r="Y7" s="14">
         <v>6560800</v>
       </c>
       <c r="Z7" s="13" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
@@ -1512,11 +1520,11 @@
       <c r="X8" s="10">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y8">
+      <c r="Y8" s="14">
         <v>6560800</v>
       </c>
       <c r="Z8" s="13" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
@@ -1594,11 +1602,11 @@
       <c r="X9">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y9">
+      <c r="Y9" s="14">
         <v>6560800</v>
       </c>
       <c r="Z9" s="13" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
@@ -1680,7 +1688,7 @@
         <v>6560800</v>
       </c>
       <c r="Z10" s="13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
@@ -1758,11 +1766,11 @@
       <c r="X11" s="10">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y11">
+      <c r="Y11" s="14">
         <v>6560800</v>
       </c>
       <c r="Z11" s="13" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
@@ -1840,11 +1848,11 @@
       <c r="X12">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y12">
+      <c r="Y12" s="14">
         <v>6560800</v>
       </c>
       <c r="Z12" s="13" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
@@ -1922,11 +1930,11 @@
       <c r="X13">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y13">
+      <c r="Y13" s="14">
         <v>6560800</v>
       </c>
       <c r="Z13" s="13" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
@@ -2008,7 +2016,7 @@
         <v>6560800</v>
       </c>
       <c r="Z14" s="13" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
@@ -2090,7 +2098,7 @@
         <v>6560800</v>
       </c>
       <c r="Z15" s="13" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
@@ -2172,7 +2180,7 @@
         <v>6560800</v>
       </c>
       <c r="Z16" s="13" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
@@ -2254,7 +2262,7 @@
         <v>6560800</v>
       </c>
       <c r="Z17" s="13" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
@@ -2336,7 +2344,7 @@
         <v>6560800</v>
       </c>
       <c r="Z18" s="13" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
@@ -2418,7 +2426,7 @@
         <v>6560800</v>
       </c>
       <c r="Z19" s="13" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
@@ -2500,7 +2508,7 @@
         <v>6560800</v>
       </c>
       <c r="Z20" s="13" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
@@ -2582,7 +2590,7 @@
         <v>6560800</v>
       </c>
       <c r="Z21" s="13" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
@@ -2664,7 +2672,7 @@
         <v>6560800</v>
       </c>
       <c r="Z22" s="13" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
@@ -2746,7 +2754,7 @@
         <v>6560800</v>
       </c>
       <c r="Z23" s="13" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
@@ -2828,7 +2836,7 @@
         <v>6560800</v>
       </c>
       <c r="Z24" s="13" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
@@ -2910,7 +2918,7 @@
         <v>6560800</v>
       </c>
       <c r="Z25" s="13" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
@@ -2988,11 +2996,11 @@
       <c r="X26" s="10">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y26">
+      <c r="Y26" s="14">
         <v>6560800</v>
       </c>
       <c r="Z26" s="13" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
@@ -3070,11 +3078,11 @@
       <c r="X27">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y27">
+      <c r="Y27" s="14">
         <v>6560800</v>
       </c>
       <c r="Z27" s="13" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
@@ -3156,7 +3164,7 @@
         <v>6560800</v>
       </c>
       <c r="Z28" s="13" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
@@ -3238,7 +3246,7 @@
         <v>6560800</v>
       </c>
       <c r="Z29" s="13" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.2">
@@ -3320,7 +3328,7 @@
         <v>6560800</v>
       </c>
       <c r="Z30" s="13" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
@@ -3402,7 +3410,7 @@
         <v>6560800</v>
       </c>
       <c r="Z31" s="13" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
@@ -3484,7 +3492,7 @@
         <v>6560800</v>
       </c>
       <c r="Z32" s="13" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
@@ -3566,7 +3574,7 @@
         <v>6560800</v>
       </c>
       <c r="Z33" s="13" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
@@ -3648,7 +3656,7 @@
         <v>6560800</v>
       </c>
       <c r="Z34" s="13" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
@@ -3730,7 +3738,7 @@
         <v>6560800</v>
       </c>
       <c r="Z35" s="13" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
@@ -3812,7 +3820,7 @@
         <v>6560800</v>
       </c>
       <c r="Z36" s="13" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
@@ -3890,11 +3898,11 @@
       <c r="X37">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y37">
+      <c r="Y37" s="14">
         <v>6560800</v>
       </c>
       <c r="Z37" s="13" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
@@ -3976,7 +3984,7 @@
         <v>6560800</v>
       </c>
       <c r="Z38" s="13" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
@@ -4054,11 +4062,11 @@
       <c r="X39">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y39">
+      <c r="Y39" s="14">
         <v>6560800</v>
       </c>
       <c r="Z39" s="13" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
@@ -4140,7 +4148,7 @@
         <v>6560800</v>
       </c>
       <c r="Z40" s="13" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
@@ -4218,11 +4226,11 @@
       <c r="X41" s="10">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y41">
+      <c r="Y41" s="14">
         <v>6560800</v>
       </c>
       <c r="Z41" s="13" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
@@ -4300,11 +4308,11 @@
       <c r="X42">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y42">
+      <c r="Y42" s="14">
         <v>6560800</v>
       </c>
       <c r="Z42" s="13" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
@@ -4386,7 +4394,7 @@
         <v>6560800</v>
       </c>
       <c r="Z43" s="13" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
@@ -4464,11 +4472,11 @@
       <c r="X44" s="10">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y44">
+      <c r="Y44" s="14">
         <v>6560800</v>
       </c>
       <c r="Z44" s="13" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
@@ -4546,11 +4554,11 @@
       <c r="X45">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y45">
+      <c r="Y45" s="14">
         <v>6560800</v>
       </c>
       <c r="Z45" s="13" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
@@ -4632,7 +4640,7 @@
         <v>6560800</v>
       </c>
       <c r="Z46" s="13" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
@@ -4710,11 +4718,11 @@
       <c r="X47" s="10">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y47">
+      <c r="Y47" s="14">
         <v>6560800</v>
       </c>
       <c r="Z47" s="13" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
@@ -4792,11 +4800,11 @@
       <c r="X48">
         <v>18.079999999999998</v>
       </c>
-      <c r="Y48">
+      <c r="Y48" s="14">
         <v>6560800</v>
       </c>
       <c r="Z48" s="13" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
@@ -4878,7 +4886,7 @@
         <v>6560800</v>
       </c>
       <c r="Z49" s="13" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
@@ -4960,7 +4968,7 @@
         <v>6560800</v>
       </c>
       <c r="Z50" s="13" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
@@ -5042,60 +5050,82 @@
         <v>6560800</v>
       </c>
       <c r="Z51" s="13" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="Z2" r:id="rId1" xr:uid="{CC65568E-1147-F840-B0C0-2E4A72C1AA3F}"/>
     <hyperlink ref="Z3" r:id="rId2" xr:uid="{889DF3FF-C593-EF42-B23E-9D730B3DDAE8}"/>
-    <hyperlink ref="Z5" r:id="rId3" xr:uid="{57BBD8F3-4E12-454E-B2F5-5F7EECE0F734}"/>
-    <hyperlink ref="Z6" r:id="rId4" xr:uid="{14641ABD-FFF3-2A43-8B39-B2A0F1A498AF}"/>
-    <hyperlink ref="Z7" r:id="rId5" xr:uid="{F974F437-7576-5D40-A751-E61296394C1A}"/>
-    <hyperlink ref="Z8" r:id="rId6" xr:uid="{7863CA1E-B0ED-0046-BDD3-C2ACB126776E}"/>
-    <hyperlink ref="Z9" r:id="rId7" display="https://www.google.com/maps/place/2612+Monticello+Ave,+Norfolk,+VA+23517/@36.8706106,-76.282217,3a,75y,26.37h,89.1t/data=!3m7!1e1!3m5!1sJm_WmtqCPNdIJ5VpTd1Abw!2e0!6s%2F%2Fgeo2.ggpht.com%2Fcbk%3Fpanoid%3DJm_WmtqCPNdIJ5VpTd1Abw%26output%3Dthumbnail%26cb_client%3Dsearch.gws-prod.gps%26thumb%3D2%26w%3D86%26h%3D86%26yaw%3D357.51123%26pitch%3D0%26thumbfov%3D100!7i13312!8i6656!4m5!3m4!1s0x89ba98254e888bd5:0xd3314741a1a16105!8m2!3d36.8707309!4d-76.282256" xr:uid="{54BAEAD7-7D61-BA4F-B0C9-79C1ECDF9458}"/>
-    <hyperlink ref="Z10" r:id="rId8" xr:uid="{A961C95B-5F01-CC40-A26A-1A9B0AFC6236}"/>
-    <hyperlink ref="Z11" r:id="rId9" xr:uid="{21E04B7A-E032-FD43-9F68-229EFC268448}"/>
-    <hyperlink ref="Z12" r:id="rId10" xr:uid="{53FAB03F-0E9D-5B47-965D-0AF28446A900}"/>
-    <hyperlink ref="Z13" r:id="rId11" xr:uid="{CED9E9D1-0E49-6C47-A94F-E7F895CB67D5}"/>
-    <hyperlink ref="Z14" r:id="rId12" xr:uid="{1912C2E0-0E18-EC44-99FE-A8A834C6829F}"/>
-    <hyperlink ref="Z15" r:id="rId13" xr:uid="{6EB57345-9596-9E48-A10C-ED041A10FF8D}"/>
-    <hyperlink ref="Z16" r:id="rId14" xr:uid="{A6CB7645-AA7A-8441-A0E9-5FACB37EC252}"/>
-    <hyperlink ref="Z17" r:id="rId15" xr:uid="{ED19529A-B3E6-7949-AEF5-812665BF2989}"/>
-    <hyperlink ref="Z18" r:id="rId16" xr:uid="{BB9141D0-7A45-B345-8390-0B1B391BD9D1}"/>
-    <hyperlink ref="Z19" r:id="rId17" xr:uid="{AFD54806-0E91-C442-A01E-BBD516091F06}"/>
-    <hyperlink ref="Z20" r:id="rId18" xr:uid="{0CE0F760-46BA-5840-9E17-CF6BDA643FB5}"/>
-    <hyperlink ref="Z21" r:id="rId19" xr:uid="{BFAE1ABD-BA6E-3C44-A76E-77DD5763D5B1}"/>
-    <hyperlink ref="Z22" r:id="rId20" xr:uid="{B12F913F-F6D6-9A4F-ACE2-0A197BD3C003}"/>
-    <hyperlink ref="Z23" r:id="rId21" xr:uid="{4C6FB7BC-22C5-7F49-BF9A-97693FB6FA19}"/>
-    <hyperlink ref="Z24" r:id="rId22" xr:uid="{5A53C554-5AA9-9549-BD2B-488160CEAE1C}"/>
-    <hyperlink ref="Z25" r:id="rId23" xr:uid="{6F5736BA-3CD6-7D40-A587-AABED8664773}"/>
-    <hyperlink ref="Z26" r:id="rId24" xr:uid="{179B7FFC-694C-1947-B262-C685D2712F9A}"/>
-    <hyperlink ref="Z27" r:id="rId25" display="https://www.google.com/maps/place/930+E+Virginia+Beach+Blvd,+Norfolk,+VA+23504/@36.8546596,-76.2749356,3a,90y,358.8h,87.93t/data=!3m6!1e1!3m4!1so68-ruh7cZGBxnC2c5gdDw!2e0!7i16384!8i8192!4m5!3m4!1s0x89ba981e9a18a563:0xfed0c4efcdd81481!8m2!3d36.855462!4d-76.27504" xr:uid="{D76F0EEF-3737-054C-884C-42F360D69182}"/>
-    <hyperlink ref="Z28" r:id="rId26" xr:uid="{B3F930B8-B0BE-3D4F-B273-D49E958C9CCD}"/>
-    <hyperlink ref="Z29" r:id="rId27" xr:uid="{F8940D37-5456-6744-A985-A414EA765364}"/>
-    <hyperlink ref="Z30" r:id="rId28" xr:uid="{9DCA8CA1-7E60-8A4C-958C-B5E164191455}"/>
-    <hyperlink ref="Z31" r:id="rId29" xr:uid="{9A28F3BE-92A4-AC47-AEC1-0A3DF6EC4780}"/>
-    <hyperlink ref="Z32" r:id="rId30" xr:uid="{520ABAD2-608C-1543-B6D3-9B5007FCD5ED}"/>
-    <hyperlink ref="Z33" r:id="rId31" xr:uid="{10BD221B-ADA4-6E4F-924C-7E545FFFE265}"/>
-    <hyperlink ref="Z34" r:id="rId32" xr:uid="{C99DD571-EBF0-F14B-87C6-3940605855C0}"/>
-    <hyperlink ref="Z35" r:id="rId33" xr:uid="{7DA24D2F-51E3-B140-A772-B31C0ECE788C}"/>
-    <hyperlink ref="Z36" r:id="rId34" xr:uid="{55F1F4A1-4566-6940-A605-9B7C4EB29F79}"/>
-    <hyperlink ref="Z37" r:id="rId35" display="https://www.google.com/maps/@36.9158979,-76.2631474,3a,75y,359h,86.4t/data=!3m7!1e1!3m5!1sQlaeuGuu5OwZHIxyA_TW7g!2e0!6s%2F%2Fgeo3.ggpht.com%2Fcbk%3Fpanoid%3DQlaeuGuu5OwZHIxyA_TW7g%26output%3Dthumbnail%26cb_client%3Dmaps_sv.tactile.gps%26thumb%3D2%26w%3D203%26h%3D100%26yaw%3D292.73462%26pitch%3D0%26thumbfov%3D100!7i16384!8i8192" xr:uid="{6B98EDBC-CA70-954E-8A54-F9D600B23465}"/>
-    <hyperlink ref="Z38" r:id="rId36" xr:uid="{B0605F8F-FD1B-EC40-8624-8A15235982CD}"/>
-    <hyperlink ref="Z39" r:id="rId37" xr:uid="{FBD3B614-ECB2-F64E-B38C-6684651669B1}"/>
-    <hyperlink ref="Z40" r:id="rId38" xr:uid="{77A9EAAD-0E58-944E-A67C-06AC6745C227}"/>
-    <hyperlink ref="Z41" r:id="rId39" xr:uid="{B5C59B50-8890-2D44-A02B-8DF7289CDF2E}"/>
-    <hyperlink ref="Z42" r:id="rId40" display="https://www.google.com/maps/place/1418+Ballentine+Blvd,+Norfolk,+VA+23504/@36.8593939,-76.2496023,3a,74.9y,75.18h,99.64t/data=!3m7!1e1!3m5!1sfWED1BsjWb_y3zyUmXEbUg!2e0!6s%2F%2Fgeo3.ggpht.com%2Fcbk%3Fpanoid%3DfWED1BsjWb_y3zyUmXEbUg%26output%3Dthumbnail%26cb_client%3Dsearch.gws-prod.gps%26thumb%3D2%26w%3D86%26h%3D86%26yaw%3D74.78842%26pitch%3D0%26thumbfov%3D100!7i16384!8i8192!4m5!3m4!1s0x89ba97959d6de8f5:0x2b0cbdf6cc0bf3fa!8m2!3d36.85963!4d-76.249023" xr:uid="{3B7A9FE8-A996-6246-9A15-178B3E87179A}"/>
-    <hyperlink ref="Z43" r:id="rId41" xr:uid="{22ACD08E-3F6B-4245-B25E-CCE7BC6C6011}"/>
-    <hyperlink ref="Z44" r:id="rId42" xr:uid="{ADB94313-FF1E-7A4E-BF8C-FF65FB291BD0}"/>
-    <hyperlink ref="Z45" r:id="rId43" xr:uid="{F902DCB2-133D-534D-A136-CAED3A3B9525}"/>
-    <hyperlink ref="Z46" r:id="rId44" xr:uid="{E83B887C-9A40-D24F-8565-01BE9A412F25}"/>
-    <hyperlink ref="Z47" r:id="rId45" xr:uid="{2FFBFFC5-E3FD-B143-AD3E-D26CE0E8C40B}"/>
-    <hyperlink ref="Z48" r:id="rId46" xr:uid="{DE6E4551-DC87-CD48-9390-B67A9BDBE3BC}"/>
-    <hyperlink ref="Z49" r:id="rId47" xr:uid="{8F54C692-48EC-0845-953C-15BE98061ECD}"/>
-    <hyperlink ref="Z50" r:id="rId48" xr:uid="{208E007F-35DF-BD45-9638-D073024D3793}"/>
-    <hyperlink ref="Z51" r:id="rId49" xr:uid="{425AC6D0-649C-A946-B067-C4FF68E6E50A}"/>
+    <hyperlink ref="Z6" r:id="rId3" xr:uid="{14641ABD-FFF3-2A43-8B39-B2A0F1A498AF}"/>
+    <hyperlink ref="Z10" r:id="rId4" xr:uid="{A961C95B-5F01-CC40-A26A-1A9B0AFC6236}"/>
+    <hyperlink ref="Z14" r:id="rId5" xr:uid="{1912C2E0-0E18-EC44-99FE-A8A834C6829F}"/>
+    <hyperlink ref="Z15" r:id="rId6" xr:uid="{6EB57345-9596-9E48-A10C-ED041A10FF8D}"/>
+    <hyperlink ref="Z16" r:id="rId7" xr:uid="{A6CB7645-AA7A-8441-A0E9-5FACB37EC252}"/>
+    <hyperlink ref="Z17" r:id="rId8" xr:uid="{ED19529A-B3E6-7949-AEF5-812665BF2989}"/>
+    <hyperlink ref="Z18" r:id="rId9" xr:uid="{BB9141D0-7A45-B345-8390-0B1B391BD9D1}"/>
+    <hyperlink ref="Z19" r:id="rId10" xr:uid="{AFD54806-0E91-C442-A01E-BBD516091F06}"/>
+    <hyperlink ref="Z20" r:id="rId11" xr:uid="{0CE0F760-46BA-5840-9E17-CF6BDA643FB5}"/>
+    <hyperlink ref="Z21" r:id="rId12" xr:uid="{BFAE1ABD-BA6E-3C44-A76E-77DD5763D5B1}"/>
+    <hyperlink ref="Z22" r:id="rId13" xr:uid="{B12F913F-F6D6-9A4F-ACE2-0A197BD3C003}"/>
+    <hyperlink ref="Z23" r:id="rId14" xr:uid="{4C6FB7BC-22C5-7F49-BF9A-97693FB6FA19}"/>
+    <hyperlink ref="Z24" r:id="rId15" xr:uid="{5A53C554-5AA9-9549-BD2B-488160CEAE1C}"/>
+    <hyperlink ref="Z25" r:id="rId16" xr:uid="{6F5736BA-3CD6-7D40-A587-AABED8664773}"/>
+    <hyperlink ref="Z28" r:id="rId17" xr:uid="{B3F930B8-B0BE-3D4F-B273-D49E958C9CCD}"/>
+    <hyperlink ref="Z29" r:id="rId18" xr:uid="{F8940D37-5456-6744-A985-A414EA765364}"/>
+    <hyperlink ref="Z30" r:id="rId19" xr:uid="{9DCA8CA1-7E60-8A4C-958C-B5E164191455}"/>
+    <hyperlink ref="Z31" r:id="rId20" xr:uid="{9A28F3BE-92A4-AC47-AEC1-0A3DF6EC4780}"/>
+    <hyperlink ref="Z32" r:id="rId21" xr:uid="{520ABAD2-608C-1543-B6D3-9B5007FCD5ED}"/>
+    <hyperlink ref="Z33" r:id="rId22" xr:uid="{10BD221B-ADA4-6E4F-924C-7E545FFFE265}"/>
+    <hyperlink ref="Z34" r:id="rId23" xr:uid="{C99DD571-EBF0-F14B-87C6-3940605855C0}"/>
+    <hyperlink ref="Z35" r:id="rId24" xr:uid="{7DA24D2F-51E3-B140-A772-B31C0ECE788C}"/>
+    <hyperlink ref="Z36" r:id="rId25" xr:uid="{55F1F4A1-4566-6940-A605-9B7C4EB29F79}"/>
+    <hyperlink ref="Z38" r:id="rId26" xr:uid="{B0605F8F-FD1B-EC40-8624-8A15235982CD}"/>
+    <hyperlink ref="Z40" r:id="rId27" xr:uid="{77A9EAAD-0E58-944E-A67C-06AC6745C227}"/>
+    <hyperlink ref="Z43" r:id="rId28" xr:uid="{22ACD08E-3F6B-4245-B25E-CCE7BC6C6011}"/>
+    <hyperlink ref="Z46" r:id="rId29" xr:uid="{E83B887C-9A40-D24F-8565-01BE9A412F25}"/>
+    <hyperlink ref="Z49" r:id="rId30" xr:uid="{8F54C692-48EC-0845-953C-15BE98061ECD}"/>
+    <hyperlink ref="Z50" r:id="rId31" xr:uid="{208E007F-35DF-BD45-9638-D073024D3793}"/>
+    <hyperlink ref="Z51" r:id="rId32" xr:uid="{425AC6D0-649C-A946-B067-C4FF68E6E50A}"/>
+    <hyperlink ref="Z11" r:id="rId33" xr:uid="{B561DED3-50A3-7A44-AFA0-B4C244DD25DB}"/>
+    <hyperlink ref="Z12" r:id="rId34" xr:uid="{38F28D88-005E-A041-ABE4-1328AC8441D3}"/>
+    <hyperlink ref="Z26" r:id="rId35" xr:uid="{95EA1FB0-FE4A-9440-B731-4208603F5B9E}"/>
+    <hyperlink ref="Z27" r:id="rId36" xr:uid="{2DA0905B-61D9-AD46-8ABC-C95BC7F94DBE}"/>
+    <hyperlink ref="Z37" r:id="rId37" xr:uid="{BE02767C-A9D3-0547-A515-AAB07E734B41}"/>
+    <hyperlink ref="Z39" r:id="rId38" xr:uid="{2AC9A84E-96CC-F84A-AC0A-64CCC9BE309D}"/>
+    <hyperlink ref="Z41" r:id="rId39" xr:uid="{1DC41A9B-3871-8743-8883-84D283302975}"/>
+    <hyperlink ref="Z42" r:id="rId40" xr:uid="{5BBDB006-59EA-7D45-BF45-F9BED8A0ED23}"/>
+    <hyperlink ref="Z44" r:id="rId41" xr:uid="{E8A91C7B-E16C-EF41-B8FF-F69E6B1CF379}"/>
+    <hyperlink ref="Z45" r:id="rId42" xr:uid="{11796B04-D07F-5342-BBCE-D34A23B8F700}"/>
+    <hyperlink ref="Z47" r:id="rId43" xr:uid="{49632334-1266-0E49-80F0-49C82D12C563}"/>
+    <hyperlink ref="Z48" r:id="rId44" xr:uid="{C3BA1CF9-EFCF-9F44-87D3-9ABA30330CA1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CEEFF04-967A-5A47-8133-F8F496213784}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{7E5F2A03-0DD9-FD4B-A1A2-C326C02B5D73}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update google map links
</commit_message>
<xml_diff>
--- a/data/addresses.xlsx
+++ b/data/addresses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbuck/Desktop/NMP/MAP673/BlightedToBountiful/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B9869C-9ABB-8748-A12B-ED3696298CA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C87E7AC-F800-2441-BDC0-E196E9EBC699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{9123AF10-BEF5-F743-AFF6-F8B1E991249B}"/>
   </bookViews>
@@ -267,99 +267,6 @@
     <t>totalValue</t>
   </si>
   <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.3114205399744&amp;y=36.8988987942398</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.308684341667&amp;y=36.8791583084625</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2975126025031&amp;y=36.8746790155474</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2723602254643&amp;y=36.8579139694955</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2760430047947&amp;y=36.8629540468538</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2737005641496&amp;y=36.863306999836</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2735996253383&amp;y=36.8633223252972</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2760134714972&amp;y=36.8655330384462</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.27347970269&amp;y=36.863964430452</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2748881317705&amp;y=36.8653543958251</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2721957489548&amp;y=36.8647407165717</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2710393633396&amp;y=36.8639233669225</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2656637997019&amp;y=36.8575645064382</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.252663659953&amp;y=36.8525912616126</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2525436931686&amp;y=36.8521261987788</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2501842085679&amp;y=36.8632022029132</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2360274134914&amp;y=36.842695430223</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2481745676197&amp;y=36.8780896254006</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2643897899723&amp;y=36.9183880904979</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2634692523333&amp;y=36.9178419464133</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2630892186519&amp;y=36.9178532197873</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2642278245403&amp;y=36.9174679787259</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2638239450241&amp;y=36.9174828028331</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.262616655931&amp;y=36.9168803738438</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2950852234906&amp;y=36.9164763650166</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2912710468707&amp;y=36.8742703307802</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2480788400734&amp;y=36.878018532031</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.263639502536&amp;y=36.9174739008572</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2648470984892&amp;y=36.916414116563</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2640990859522&amp;y=36.9163391766515</t>
-  </si>
-  <si>
-    <t>https://air.norfolk.gov/allimagery/streetview.html?x=-76.2643907525144&amp;y=36.9163664359159</t>
-  </si>
-  <si>
     <t>streetView</t>
   </si>
   <si>
@@ -418,6 +325,99 @@
   </si>
   <si>
     <t>https://www.google.com/maps/embed?pb=!4v1591900531258!6m8!1m7!1sn02BncmaPSzSnv5Bc6oXRg!2m2!1d36.91605702410043!2d-76.26479426860529!3f20.16!4f5.189999999999998!5f0.7820865974627469</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592665065170!6m8!1m7!1sMouHbQNkfq1KxzhNbKlxfg!2m2!1d36.89904235162321!2d-76.3114980328535!3f157.09!4f10.400000000000006!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592665172692!6m8!1m7!1s-tCUM7tirQ1gU2se5Vkymw!2m2!1d36.87941427509518!2d-76.30873123639898!3f171.66!4f10!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592665234801!6m8!1m7!1sR00yvp93G_GbsISBr5Uxqg!2m2!1d36.87457631912579!2d-76.29724063682792!3f289.46395626850057!4f-6.911394967165293!5f0.4000000000000002</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592665335209!6m8!1m7!1sO5Egiw4IOB1_r1tu4BWFwA!2m2!1d36.85804139313613!2d-76.27273965538782!3f116.88!4f10.120000000000005!5f0.4000000000000002</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592665502514!6m8!1m7!1seBOvGINkRVe6370BDQEVbA!2m2!1d36.86314790329126!2d-76.27614736218922!3f168.34985944483896!4f5.958496962112932!5f0.772798507860903</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592665674872!6m8!1m7!1sCIA3gXXlK8Erlc2ceG4Vhw!2m2!1d36.86350246537197!2d-76.27355274908923!3f165.71932234716053!4f9.303222430462228!5f0.4000000000000002</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592665715906!6m8!1m7!1swxl7W_svb4ZWQ9m0EalZxw!2m2!1d36.86348702612092!2d-76.27366095485304!3f163.41!4f10!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592665802086!6m8!1m7!1siBiQv1U88xQo56FPN0bTbw!2m2!1d36.8653228629351!2d-76.27600445696524!3f354.71864308642256!4f17.18177817873854!5f0.6222866636070421</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592665866558!6m8!1m7!1sK8CIvENU77mgE5vtfrZV1Q!2m2!1d36.86407357873125!2d-76.27335722979419!3f226.3629951882023!4f6.272487650330447!5f0.40457075809216086</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592665910517!6m8!1m7!1sEOjj2zmBL_8aVmC6UzbDXA!2m2!1d36.86547768723604!2d-76.27491296817067!3f148.13217185869334!4f3.43206204996757!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592665965000!6m8!1m7!1sQ1I0oMD2odkZEZ1PXIB6ZA!2m2!1d36.86452796795547!2d-76.2723941379832!3f45.99038225872033!4f12.969750919508996!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592666012188!6m8!1m7!1sfPG6cEeUFEdTGJomKGKTng!2m2!1d36.86376641053696!2d-76.27121155879614!3f41.27!4f10!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592666051032!6m8!1m7!1sCG3Ng0Hx8RZEQ13yLzrYig!2m2!1d36.85762740240267!2d-76.26594294015538!3f105.73!4f10!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592666090791!6m8!1m7!1sT_es5p9pD31t-YdcIFDQ3w!2m2!1d36.85262526672637!2d-76.25288425539694!3f93.08!4f5.280000000000001!5f0.4000000000000002</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592666132074!6m8!1m7!1sRuz1hRa0iLnmbPUVE859-w!2m2!1d36.85231287239939!2d-76.25259655463324!3f175.0958478974717!4f13.479749444927066!5f0.4000000000000002</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592666601823!6m8!1m7!1sCb2GYi55avnnrzEDyGWizQ!2m2!1d36.86315019098656!2d-76.25047304898814!3f80.03128482601167!4f16.304269243189196!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592666660733!6m8!1m7!1szX0TfVNGZLmCf7OzWxMAdg!2m2!1d36.84289222935679!2d-76.23597456947694!3f190.29873437114486!4f1.9053999445556684!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592666719772!6m8!1m7!1sgefwOVajIVpFF49p8o8dLw!2m2!1d36.87819215425838!2d-76.2480911662013!3f196.67710380758538!4f10.889840812576509!5f0.4000000000000002</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592666778575!6m8!1m7!1sGdcC0h8tp6KS7HmIkGOAQQ!2m2!1d36.91809792339702!2d-76.26426239307821!3f338.4674807008512!4f11.219220755293307!5f0.7876917578202689</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592666820888!6m8!1m7!1syOXh5P2YAc0EgmMU_szb3Q!2m2!1d36.91809581220794!2d-76.26349290489136!3f179.9333766983505!4f9.991950961987811!5f0.5586361636509503</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592666877268!6m8!1m7!1sGG_LLEJcrlPic7Dv-GbKmw!2m2!1d36.91812480341552!2d-76.2630478571323!3f189.25068923950414!4f6.130099650796822!5f0.415847888206226</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592666912681!6m8!1m7!1sEEsgn4M4w19lv5nJF3RpeQ!2m2!1d36.91729288221892!2d-76.26423205359693!3f1.11!4f10!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592666950210!6m8!1m7!1skJY0XlTFcvK4V4NYPbrEYA!2m2!1d36.91725404602425!2d-76.26384721333136!3f6.87!4f19.58!5f0.4000000000000002</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592667188917!6m8!1m7!1sJMPFSuRfSSvseozxtvMYtw!2m2!1d36.91714325084339!2d-76.26257363155776!3f194.96679944940217!4f10.082113883271404!5f0.4516936881563587</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592667227532!6m8!1m7!1s_N82mesAxnrX91JXeeRgeQ!2m2!1d36.91679721300318!2d-76.2951005920984!3f178.0699692599674!4f10.455795409990998!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592667268960!6m8!1m7!1s-ejLgWnhuKiKXgscOvPtPQ!2m2!1d36.8743018445842!2d-76.29140445175926!3f103.43!4f11.790000000000006!5f0.4000000000000002</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592667311839!6m8!1m7!1scQWWfGHswCQSKBY0YVFrpg!2m2!1d36.87815689266255!2d-76.24798190046953!3f209.43!4f17.019999999999996!5f0.4000000000000002</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592667376459!6m8!1m7!1s73rkJmwZ2ho91UnTOCd-KQ!2m2!1d36.91724356474509!2d-76.26373672751919!3f2.297877136421069!4f5.549315654572695!5f0.40435055844788387</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592667410618!6m8!1m7!1swKtNmFyou0we7Rx09QZyYA!2m2!1d36.91617068400947!2d-76.26509212568918!3f38.83!4f10!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592667450549!6m8!1m7!1sbsjZO5OJ8v4P0ZLRK-dbEg!2m2!1d36.91598266032241!2d-76.26413338658887!3f4.4!4f10!5f0.8160813932612223</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!4v1592667492286!6m8!1m7!1sZLzWDRJdX5fCrRxvPna0AA!2m2!1d36.91602678859328!2d-76.26446360364872!3f9.73!4f10!5f0.8160813932612223</t>
   </si>
 </sst>
 </file>
@@ -857,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33098549-00A6-B548-BC6F-D00EF842369B}">
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Y48" sqref="Y48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -950,7 +950,7 @@
         <v>76</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -1032,7 +1032,7 @@
         <v>6560800</v>
       </c>
       <c r="Z2" s="13" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -1114,7 +1114,7 @@
         <v>6560800</v>
       </c>
       <c r="Z3" s="13" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
@@ -1196,7 +1196,7 @@
         <v>6560800</v>
       </c>
       <c r="Z4" s="13" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
@@ -1278,7 +1278,7 @@
         <v>6560800</v>
       </c>
       <c r="Z5" s="13" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
@@ -1360,7 +1360,7 @@
         <v>6560800</v>
       </c>
       <c r="Z6" s="13" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
@@ -1442,7 +1442,7 @@
         <v>6560800</v>
       </c>
       <c r="Z7" s="13" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
@@ -1524,7 +1524,7 @@
         <v>6560800</v>
       </c>
       <c r="Z8" s="13" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
@@ -1606,7 +1606,7 @@
         <v>6560800</v>
       </c>
       <c r="Z9" s="13" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
@@ -1688,7 +1688,7 @@
         <v>6560800</v>
       </c>
       <c r="Z10" s="13" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
@@ -1770,7 +1770,7 @@
         <v>6560800</v>
       </c>
       <c r="Z11" s="13" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
@@ -1852,7 +1852,7 @@
         <v>6560800</v>
       </c>
       <c r="Z12" s="13" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
@@ -1934,7 +1934,7 @@
         <v>6560800</v>
       </c>
       <c r="Z13" s="13" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
@@ -2016,7 +2016,7 @@
         <v>6560800</v>
       </c>
       <c r="Z14" s="13" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
@@ -2098,7 +2098,7 @@
         <v>6560800</v>
       </c>
       <c r="Z15" s="13" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
@@ -2180,7 +2180,7 @@
         <v>6560800</v>
       </c>
       <c r="Z16" s="13" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
@@ -2262,7 +2262,7 @@
         <v>6560800</v>
       </c>
       <c r="Z17" s="13" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
@@ -2344,7 +2344,7 @@
         <v>6560800</v>
       </c>
       <c r="Z18" s="13" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
@@ -2426,7 +2426,7 @@
         <v>6560800</v>
       </c>
       <c r="Z19" s="13" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
@@ -2508,7 +2508,7 @@
         <v>6560800</v>
       </c>
       <c r="Z20" s="13" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
@@ -2590,7 +2590,7 @@
         <v>6560800</v>
       </c>
       <c r="Z21" s="13" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
@@ -2672,7 +2672,7 @@
         <v>6560800</v>
       </c>
       <c r="Z22" s="13" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
@@ -2754,7 +2754,7 @@
         <v>6560800</v>
       </c>
       <c r="Z23" s="13" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
@@ -2836,7 +2836,7 @@
         <v>6560800</v>
       </c>
       <c r="Z24" s="13" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
@@ -2918,7 +2918,7 @@
         <v>6560800</v>
       </c>
       <c r="Z25" s="13" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
@@ -3000,7 +3000,7 @@
         <v>6560800</v>
       </c>
       <c r="Z26" s="13" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
@@ -3082,7 +3082,7 @@
         <v>6560800</v>
       </c>
       <c r="Z27" s="13" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
@@ -3164,7 +3164,7 @@
         <v>6560800</v>
       </c>
       <c r="Z28" s="13" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
@@ -3246,7 +3246,7 @@
         <v>6560800</v>
       </c>
       <c r="Z29" s="13" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.2">
@@ -3328,7 +3328,7 @@
         <v>6560800</v>
       </c>
       <c r="Z30" s="13" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
@@ -3410,7 +3410,7 @@
         <v>6560800</v>
       </c>
       <c r="Z31" s="13" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
@@ -3492,7 +3492,7 @@
         <v>6560800</v>
       </c>
       <c r="Z32" s="13" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
@@ -3574,7 +3574,7 @@
         <v>6560800</v>
       </c>
       <c r="Z33" s="13" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
@@ -3656,7 +3656,7 @@
         <v>6560800</v>
       </c>
       <c r="Z34" s="13" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
@@ -3738,7 +3738,7 @@
         <v>6560800</v>
       </c>
       <c r="Z35" s="13" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
@@ -3820,7 +3820,7 @@
         <v>6560800</v>
       </c>
       <c r="Z36" s="13" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
@@ -3902,7 +3902,7 @@
         <v>6560800</v>
       </c>
       <c r="Z37" s="13" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
@@ -3984,7 +3984,7 @@
         <v>6560800</v>
       </c>
       <c r="Z38" s="13" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
@@ -4066,7 +4066,7 @@
         <v>6560800</v>
       </c>
       <c r="Z39" s="13" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
@@ -4148,7 +4148,7 @@
         <v>6560800</v>
       </c>
       <c r="Z40" s="13" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
@@ -4230,7 +4230,7 @@
         <v>6560800</v>
       </c>
       <c r="Z41" s="13" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
@@ -4312,7 +4312,7 @@
         <v>6560800</v>
       </c>
       <c r="Z42" s="13" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
@@ -4394,7 +4394,7 @@
         <v>6560800</v>
       </c>
       <c r="Z43" s="13" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
@@ -4476,7 +4476,7 @@
         <v>6560800</v>
       </c>
       <c r="Z44" s="13" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
@@ -4558,7 +4558,7 @@
         <v>6560800</v>
       </c>
       <c r="Z45" s="13" t="s">
-        <v>125</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
@@ -4640,7 +4640,7 @@
         <v>6560800</v>
       </c>
       <c r="Z46" s="13" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
@@ -4722,7 +4722,7 @@
         <v>6560800</v>
       </c>
       <c r="Z47" s="13" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
@@ -4804,7 +4804,7 @@
         <v>6560800</v>
       </c>
       <c r="Z48" s="13" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
@@ -4886,7 +4886,7 @@
         <v>6560800</v>
       </c>
       <c r="Z49" s="13" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
@@ -4968,7 +4968,7 @@
         <v>6560800</v>
       </c>
       <c r="Z50" s="13" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
@@ -5050,55 +5050,54 @@
         <v>6560800</v>
       </c>
       <c r="Z51" s="13" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Z2" r:id="rId1" xr:uid="{CC65568E-1147-F840-B0C0-2E4A72C1AA3F}"/>
-    <hyperlink ref="Z3" r:id="rId2" xr:uid="{889DF3FF-C593-EF42-B23E-9D730B3DDAE8}"/>
-    <hyperlink ref="Z6" r:id="rId3" xr:uid="{14641ABD-FFF3-2A43-8B39-B2A0F1A498AF}"/>
-    <hyperlink ref="Z10" r:id="rId4" xr:uid="{A961C95B-5F01-CC40-A26A-1A9B0AFC6236}"/>
-    <hyperlink ref="Z14" r:id="rId5" xr:uid="{1912C2E0-0E18-EC44-99FE-A8A834C6829F}"/>
-    <hyperlink ref="Z15" r:id="rId6" xr:uid="{6EB57345-9596-9E48-A10C-ED041A10FF8D}"/>
-    <hyperlink ref="Z16" r:id="rId7" xr:uid="{A6CB7645-AA7A-8441-A0E9-5FACB37EC252}"/>
-    <hyperlink ref="Z17" r:id="rId8" xr:uid="{ED19529A-B3E6-7949-AEF5-812665BF2989}"/>
-    <hyperlink ref="Z18" r:id="rId9" xr:uid="{BB9141D0-7A45-B345-8390-0B1B391BD9D1}"/>
-    <hyperlink ref="Z19" r:id="rId10" xr:uid="{AFD54806-0E91-C442-A01E-BBD516091F06}"/>
-    <hyperlink ref="Z20" r:id="rId11" xr:uid="{0CE0F760-46BA-5840-9E17-CF6BDA643FB5}"/>
-    <hyperlink ref="Z21" r:id="rId12" xr:uid="{BFAE1ABD-BA6E-3C44-A76E-77DD5763D5B1}"/>
-    <hyperlink ref="Z22" r:id="rId13" xr:uid="{B12F913F-F6D6-9A4F-ACE2-0A197BD3C003}"/>
-    <hyperlink ref="Z23" r:id="rId14" xr:uid="{4C6FB7BC-22C5-7F49-BF9A-97693FB6FA19}"/>
-    <hyperlink ref="Z24" r:id="rId15" xr:uid="{5A53C554-5AA9-9549-BD2B-488160CEAE1C}"/>
-    <hyperlink ref="Z25" r:id="rId16" xr:uid="{6F5736BA-3CD6-7D40-A587-AABED8664773}"/>
-    <hyperlink ref="Z28" r:id="rId17" xr:uid="{B3F930B8-B0BE-3D4F-B273-D49E958C9CCD}"/>
-    <hyperlink ref="Z29" r:id="rId18" xr:uid="{F8940D37-5456-6744-A985-A414EA765364}"/>
-    <hyperlink ref="Z30" r:id="rId19" xr:uid="{9DCA8CA1-7E60-8A4C-958C-B5E164191455}"/>
-    <hyperlink ref="Z31" r:id="rId20" xr:uid="{9A28F3BE-92A4-AC47-AEC1-0A3DF6EC4780}"/>
-    <hyperlink ref="Z32" r:id="rId21" xr:uid="{520ABAD2-608C-1543-B6D3-9B5007FCD5ED}"/>
-    <hyperlink ref="Z33" r:id="rId22" xr:uid="{10BD221B-ADA4-6E4F-924C-7E545FFFE265}"/>
-    <hyperlink ref="Z34" r:id="rId23" xr:uid="{C99DD571-EBF0-F14B-87C6-3940605855C0}"/>
-    <hyperlink ref="Z35" r:id="rId24" xr:uid="{7DA24D2F-51E3-B140-A772-B31C0ECE788C}"/>
-    <hyperlink ref="Z36" r:id="rId25" xr:uid="{55F1F4A1-4566-6940-A605-9B7C4EB29F79}"/>
-    <hyperlink ref="Z38" r:id="rId26" xr:uid="{B0605F8F-FD1B-EC40-8624-8A15235982CD}"/>
-    <hyperlink ref="Z40" r:id="rId27" xr:uid="{77A9EAAD-0E58-944E-A67C-06AC6745C227}"/>
-    <hyperlink ref="Z43" r:id="rId28" xr:uid="{22ACD08E-3F6B-4245-B25E-CCE7BC6C6011}"/>
-    <hyperlink ref="Z46" r:id="rId29" xr:uid="{E83B887C-9A40-D24F-8565-01BE9A412F25}"/>
-    <hyperlink ref="Z49" r:id="rId30" xr:uid="{8F54C692-48EC-0845-953C-15BE98061ECD}"/>
-    <hyperlink ref="Z50" r:id="rId31" xr:uid="{208E007F-35DF-BD45-9638-D073024D3793}"/>
-    <hyperlink ref="Z51" r:id="rId32" xr:uid="{425AC6D0-649C-A946-B067-C4FF68E6E50A}"/>
-    <hyperlink ref="Z11" r:id="rId33" xr:uid="{B561DED3-50A3-7A44-AFA0-B4C244DD25DB}"/>
-    <hyperlink ref="Z12" r:id="rId34" xr:uid="{38F28D88-005E-A041-ABE4-1328AC8441D3}"/>
-    <hyperlink ref="Z26" r:id="rId35" xr:uid="{95EA1FB0-FE4A-9440-B731-4208603F5B9E}"/>
-    <hyperlink ref="Z27" r:id="rId36" xr:uid="{2DA0905B-61D9-AD46-8ABC-C95BC7F94DBE}"/>
-    <hyperlink ref="Z37" r:id="rId37" xr:uid="{BE02767C-A9D3-0547-A515-AAB07E734B41}"/>
-    <hyperlink ref="Z39" r:id="rId38" xr:uid="{2AC9A84E-96CC-F84A-AC0A-64CCC9BE309D}"/>
-    <hyperlink ref="Z41" r:id="rId39" xr:uid="{1DC41A9B-3871-8743-8883-84D283302975}"/>
-    <hyperlink ref="Z42" r:id="rId40" xr:uid="{5BBDB006-59EA-7D45-BF45-F9BED8A0ED23}"/>
-    <hyperlink ref="Z44" r:id="rId41" xr:uid="{E8A91C7B-E16C-EF41-B8FF-F69E6B1CF379}"/>
-    <hyperlink ref="Z45" r:id="rId42" xr:uid="{11796B04-D07F-5342-BBCE-D34A23B8F700}"/>
-    <hyperlink ref="Z47" r:id="rId43" xr:uid="{49632334-1266-0E49-80F0-49C82D12C563}"/>
-    <hyperlink ref="Z48" r:id="rId44" xr:uid="{C3BA1CF9-EFCF-9F44-87D3-9ABA30330CA1}"/>
+    <hyperlink ref="Z6" r:id="rId1" xr:uid="{14641ABD-FFF3-2A43-8B39-B2A0F1A498AF}"/>
+    <hyperlink ref="Z11" r:id="rId2" xr:uid="{B561DED3-50A3-7A44-AFA0-B4C244DD25DB}"/>
+    <hyperlink ref="Z12" r:id="rId3" xr:uid="{38F28D88-005E-A041-ABE4-1328AC8441D3}"/>
+    <hyperlink ref="Z26" r:id="rId4" xr:uid="{95EA1FB0-FE4A-9440-B731-4208603F5B9E}"/>
+    <hyperlink ref="Z27" r:id="rId5" xr:uid="{2DA0905B-61D9-AD46-8ABC-C95BC7F94DBE}"/>
+    <hyperlink ref="Z37" r:id="rId6" xr:uid="{BE02767C-A9D3-0547-A515-AAB07E734B41}"/>
+    <hyperlink ref="Z39" r:id="rId7" xr:uid="{2AC9A84E-96CC-F84A-AC0A-64CCC9BE309D}"/>
+    <hyperlink ref="Z41" r:id="rId8" xr:uid="{1DC41A9B-3871-8743-8883-84D283302975}"/>
+    <hyperlink ref="Z42" r:id="rId9" xr:uid="{5BBDB006-59EA-7D45-BF45-F9BED8A0ED23}"/>
+    <hyperlink ref="Z44" r:id="rId10" xr:uid="{E8A91C7B-E16C-EF41-B8FF-F69E6B1CF379}"/>
+    <hyperlink ref="Z45" r:id="rId11" xr:uid="{11796B04-D07F-5342-BBCE-D34A23B8F700}"/>
+    <hyperlink ref="Z47" r:id="rId12" xr:uid="{49632334-1266-0E49-80F0-49C82D12C563}"/>
+    <hyperlink ref="Z48" r:id="rId13" xr:uid="{C3BA1CF9-EFCF-9F44-87D3-9ABA30330CA1}"/>
+    <hyperlink ref="Z3" r:id="rId14" xr:uid="{88C1F6D0-F68D-5E43-91A4-DBB139D54AD3}"/>
+    <hyperlink ref="Z10" r:id="rId15" xr:uid="{BF722989-7DFF-7646-B851-ED0059B246D5}"/>
+    <hyperlink ref="Z14" r:id="rId16" xr:uid="{8F2FE335-BDB6-8E40-863B-0D86BEA88B44}"/>
+    <hyperlink ref="Z15" r:id="rId17" xr:uid="{FEC962A3-14AD-D049-B3A4-C76BBB311BC0}"/>
+    <hyperlink ref="Z16" r:id="rId18" xr:uid="{263BE688-389B-9E43-B34D-15ECEFD05E3F}"/>
+    <hyperlink ref="Z17" r:id="rId19" xr:uid="{496B725C-DA06-DB47-9BE2-12720B03B81A}"/>
+    <hyperlink ref="Z18" r:id="rId20" xr:uid="{108BF1A6-8947-C74F-91A7-B903502176AE}"/>
+    <hyperlink ref="Z19" r:id="rId21" xr:uid="{F97C46AF-6042-D043-94FE-046A7E9F96A2}"/>
+    <hyperlink ref="Z20" r:id="rId22" xr:uid="{64F62980-3E19-E34A-BEB4-DAB90A674F1E}"/>
+    <hyperlink ref="Z21" r:id="rId23" xr:uid="{E97F42EA-C335-504B-AE8D-5527F7A164A8}"/>
+    <hyperlink ref="Z22" r:id="rId24" xr:uid="{2C67E601-9E1C-5D4B-AEF9-16EE25384589}"/>
+    <hyperlink ref="Z23" r:id="rId25" xr:uid="{FC2436BB-3DA5-354E-8283-3AF403F78F6B}"/>
+    <hyperlink ref="Z24" r:id="rId26" xr:uid="{A50C83B6-1616-B14E-9833-2D585E38549D}"/>
+    <hyperlink ref="Z25" r:id="rId27" xr:uid="{B110EE2F-2CEF-624D-BFCF-7CF90CABDD09}"/>
+    <hyperlink ref="Z28" r:id="rId28" xr:uid="{DA41D5F9-92BF-7045-8E30-EDFC6057E5C5}"/>
+    <hyperlink ref="Z29" r:id="rId29" xr:uid="{93D18C45-897E-2447-A18B-19E0F0226235}"/>
+    <hyperlink ref="Z30" r:id="rId30" xr:uid="{6C361314-FAC1-0146-AD8A-B21832ED7903}"/>
+    <hyperlink ref="Z31" r:id="rId31" xr:uid="{D3FE74AF-FBFC-2040-9C68-9CB09E225E19}"/>
+    <hyperlink ref="Z32" r:id="rId32" xr:uid="{AE10C3F2-DBC0-CD4B-896F-2181EA85F700}"/>
+    <hyperlink ref="Z33" r:id="rId33" xr:uid="{A1FBCAF2-5ABC-AC4C-B547-B8F93765F525}"/>
+    <hyperlink ref="Z34" r:id="rId34" xr:uid="{042F4D36-7FC2-CC41-962E-56592F654E50}"/>
+    <hyperlink ref="Z35" r:id="rId35" xr:uid="{98EB63E8-50A1-3545-9F64-D53C0EF42B40}"/>
+    <hyperlink ref="Z36" r:id="rId36" xr:uid="{740EA5DA-F8A3-5647-B3EB-DA2176F75E18}"/>
+    <hyperlink ref="Z38" r:id="rId37" xr:uid="{4405BAC7-E4E7-5B4B-823C-6A7CF374D158}"/>
+    <hyperlink ref="Z40" r:id="rId38" xr:uid="{6CD95481-C5C6-F241-97D0-212925FB88B7}"/>
+    <hyperlink ref="Z43" r:id="rId39" xr:uid="{A8E0BD76-133B-9341-BE41-EA2FFE542A30}"/>
+    <hyperlink ref="Z46" r:id="rId40" xr:uid="{46CF60A1-5C2B-0B43-BAB6-7E32BE039DD6}"/>
+    <hyperlink ref="Z49" r:id="rId41" xr:uid="{DF5D4CD4-F4BD-4147-960C-B32CD6950967}"/>
+    <hyperlink ref="Z50" r:id="rId42" xr:uid="{422D64DF-B21E-BF4C-89E8-085A69E76F4B}"/>
+    <hyperlink ref="Z51" r:id="rId43" xr:uid="{5FFE20EE-D1AD-D54A-95F6-5BFDFFCF1312}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5125,7 +5124,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{7E5F2A03-0DD9-FD4B-A1A2-C326C02B5D73}"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{E445DFAE-DF62-064B-9CCD-12C06D12F17D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>